<commit_message>
Added download file functionality
</commit_message>
<xml_diff>
--- a/Wednesday2.xlsx
+++ b/Wednesday2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark.mathenge\Music\LinkedIn-Social-Listening\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE79BA3F-3DAB-4547-8D42-632E885206A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B922625-E7FD-44AB-A464-7BBBC3ABC80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -699,6 +699,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -709,7 +710,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -732,11 +733,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -747,11 +844,192 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -762,6 +1040,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6AF11AF7-6091-4F44-8B59-D7DCE0AB7081}" name="Table1" displayName="Table1" ref="A1:E58" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:E58" xr:uid="{6AF11AF7-6091-4F44-8B59-D7DCE0AB7081}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{BBE05DF2-00B8-41C5-8E6E-6DB15E5C58E9}" name="Name" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{CF803AD1-DCFA-47E5-8E39-551673108270}" name="Job Title" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{A2C26F99-D77E-4B1D-A8FD-E1C58581ABFF}" name="Company Name" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{A9C6D1B5-B1E8-47C0-A4B6-40505E04F1F9}" name="Company Location" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{E200EE99-8C48-4D47-965B-653C39BBCC8F}" name="Company Employee Count" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1051,8 +1343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C12" sqref="A2:E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1066,993 +1358,996 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="6" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="A20" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="A21" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="6" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="A23" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="A25" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="6" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="A26" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="A27" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="6" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="A31" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="A32" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="A33" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="6" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="A34" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="A35" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="6" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="A36" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="A37" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="A38" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="A39" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="A40" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="A41" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="A42" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+      <c r="A43" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="A44" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="A45" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+      <c r="A46" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+      <c r="A47" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="6" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+      <c r="A48" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="6" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+      <c r="A49" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="6" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+      <c r="A50" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="6" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+      <c r="A51" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+      <c r="A52" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+      <c r="A53" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+      <c r="A54" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="6" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+      <c r="A55" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+      <c r="A56" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="6" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+      <c r="A57" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+      <c r="A58" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="12" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2060,7 +2355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>